<commit_message>
add force move effect and searcher effect
</commit_message>
<xml_diff>
--- a/Data/Config/excel/effect/effect_filters.xlsx
+++ b/Data/Config/excel/effect/effect_filters.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13650"/>
+    <workbookView windowWidth="19455" windowHeight="8550"/>
   </bookViews>
   <sheets>
     <sheet name="filter" sheetId="1" r:id="rId1"/>
@@ -203,29 +203,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -233,47 +210,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -285,6 +233,44 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -293,11 +279,26 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -309,32 +310,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -356,19 +356,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -380,121 +524,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -506,37 +536,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -547,6 +547,30 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -561,30 +585,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -608,27 +608,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -647,6 +627,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -655,10 +655,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -667,133 +667,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1151,8 +1151,8 @@
   <sheetPr/>
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1167,8 +1167,11 @@
     <col min="12" max="12" width="27.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:4">
       <c r="A1">
+        <v>11</v>
+      </c>
+      <c r="D1">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
modify and implete force move and search effect
</commit_message>
<xml_diff>
--- a/Data/Config/excel/effect/effect_filters.xlsx
+++ b/Data/Config/excel/effect/effect_filters.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19455" windowHeight="8550"/>
+    <workbookView windowWidth="27765" windowHeight="13650"/>
   </bookViews>
   <sheets>
     <sheet name="filter" sheetId="1" r:id="rId1"/>
@@ -191,8 +191,8 @@
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -211,7 +211,121 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -226,122 +340,8 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -356,187 +356,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -547,6 +547,30 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -561,6 +585,17 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -589,26 +624,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -627,26 +647,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -655,10 +655,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -667,133 +667,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1151,8 +1151,8 @@
   <sheetPr/>
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>

</xml_diff>

<commit_message>
modify auto gen config
</commit_message>
<xml_diff>
--- a/Data/Config/excel/effect/effect_filters.xlsx
+++ b/Data/Config/excel/effect/effect_filters.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21840" windowHeight="13650"/>
+    <workbookView windowWidth="27765" windowHeight="13650"/>
   </bookViews>
   <sheets>
     <sheet name="filter" sheetId="1" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36">
   <si>
     <t>id</t>
   </si>
@@ -139,7 +139,10 @@
     <t>hero;monster;soldier;building</t>
   </si>
   <si>
-    <t>self;friend</t>
+    <t>enemy</t>
+  </si>
+  <si>
+    <t>target_pos</t>
   </si>
   <si>
     <t>away_caster</t>
@@ -151,6 +154,9 @@
     <t>self;enemy</t>
   </si>
   <si>
+    <t>target_unit</t>
+  </si>
+  <si>
     <t>10;10</t>
   </si>
   <si>
@@ -160,36 +166,29 @@
     <t>self</t>
   </si>
   <si>
+    <t>caster</t>
+  </si>
+  <si>
     <t>10;90</t>
   </si>
   <si>
     <t>away_target</t>
   </si>
   <si>
-    <t>enemy</t>
-  </si>
-  <si>
-    <t>target_pos</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>target_unit</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>caster</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>effect_target_unit</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -198,32 +197,345 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="9"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="9"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="9"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -231,9 +543,251 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -242,10 +796,57 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -536,19 +1137,19 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="16.625" customWidth="1"/>
     <col min="2" max="6" width="36" customWidth="1"/>
@@ -560,7 +1161,7 @@
     <col min="12" max="12" width="27.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4">
       <c r="A1">
         <v>11</v>
       </c>
@@ -568,7 +1169,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -597,7 +1198,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -626,7 +1227,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -655,7 +1256,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>1000001</v>
       </c>
@@ -672,13 +1273,13 @@
         <v>23</v>
       </c>
       <c r="F13" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="G13">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:8">
       <c r="A14">
         <v>1000002</v>
       </c>
@@ -686,25 +1287,25 @@
         <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D14" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E14" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F14" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="G14">
         <v>0</v>
       </c>
       <c r="H14" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9">
       <c r="A15">
         <v>1000003</v>
       </c>
@@ -712,25 +1313,25 @@
         <v>0</v>
       </c>
       <c r="C15" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E15" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F15" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G15">
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>1000004</v>
       </c>
@@ -738,25 +1339,25 @@
         <v>0</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D16" t="s">
         <v>22</v>
       </c>
       <c r="E16" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="F16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G16">
         <v>100</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <legacyDrawing r:id="rId1"/>
+  <headerFooter/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>